<commit_message>
Update excel version to fix H2O MW
Update H2O MW from 18 to 18.02 to match python code and webapp
</commit_message>
<xml_diff>
--- a/DensityX.xlsx
+++ b/DensityX.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovino/Dropbox/Research/_Manuscripts in Progress/DensityX Manuscript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/Calculators and Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD0AE0C-BDF5-BB4A-9B48-EE9877E5F252}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C5793C-E908-7C40-8CFA-6DE5315A9A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20580" yWindow="800" windowWidth="30620" windowHeight="18280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Density Calc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,6 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Verdana"/>
+            <family val="2"/>
           </rPr>
           <t>Kayla Iacovino:</t>
         </r>
@@ -49,6 +56,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Verdana"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Input the composition of your sample in terms of wt%
@@ -64,6 +72,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Verdana"/>
+            <family val="2"/>
           </rPr>
           <t>Kayla Iacovino:</t>
         </r>
@@ -72,6 +81,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Verdana"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -81,6 +91,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Verdana"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Vi or Vref at 1 bar at 1673K.
 </t>
@@ -90,6 +101,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Verdana"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -99,6 +111,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Verdana"/>
+            <family val="2"/>
           </rPr>
           <t>Value for H2O is from Ochs &amp; Lange 1999. Reference Conditions are 1273 K and 1 bar.</t>
         </r>
@@ -112,6 +125,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -120,6 +134,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Input sample temperature in degrees  C</t>
@@ -134,6 +149,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -142,6 +158,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -151,6 +168,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Input sample pressure in bars</t>
         </r>
@@ -273,17 +291,17 @@
     <t>Calculated automatically:</t>
   </si>
   <si>
-    <t>DensityX v1.1.0 (equivalent to Glass Density Calc v4.0)</t>
-  </si>
-  <si>
-    <t>Last updated 29 Nov 2018</t>
+    <t>Last updated 04 Apr 2023</t>
+  </si>
+  <si>
+    <t>DensityX v1.2.0 (updated molecular weight of H2O from 18 to 18.02 to match the python code and webapp)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -292,94 +310,116 @@
       <b/>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF0070C0"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFC00000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -596,8 +636,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1203,7 +1245,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="A31" sqref="A31:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1237,7 +1279,7 @@
       <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -1721,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <v>18</v>
+        <v>18.02</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="3"/>
@@ -1888,15 +1930,15 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="23"/>
+        <v>36</v>
+      </c>
+      <c r="B30" s="22"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="23"/>
+        <v>35</v>
+      </c>
+      <c r="B31" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>